<commit_message>
Adicionando areas no modelo
</commit_message>
<xml_diff>
--- a/resultados/geral_por_RM_UF.xlsx
+++ b/resultados/geral_por_RM_UF.xlsx
@@ -505,13 +505,13 @@
         <v>0.7803418803418803</v>
       </c>
       <c r="H2" t="n">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I2" t="n">
-        <v>1.512820512820513</v>
+        <v>1.51025641025641</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9897435897435898</v>
+        <v>0.9914529914529915</v>
       </c>
     </row>
     <row r="3">
@@ -539,13 +539,13 @@
         <v>0.8079922027290448</v>
       </c>
       <c r="H3" t="n">
-        <v>1169</v>
+        <v>1163</v>
       </c>
       <c r="I3" t="n">
-        <v>1.105960264900662</v>
+        <v>1.100283822138127</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9376218323586745</v>
+        <v>0.9395711500974658</v>
       </c>
     </row>
     <row r="4">
@@ -573,10 +573,10 @@
         <v>0.9086021505376344</v>
       </c>
       <c r="H4" t="n">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="I4" t="n">
-        <v>1.07258064516129</v>
+        <v>1.112903225806452</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
@@ -607,13 +607,13 @@
         <v>0.7566765578635015</v>
       </c>
       <c r="H5" t="n">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="I5" t="n">
-        <v>1.314540059347181</v>
+        <v>1.350148367952522</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9802176063303659</v>
+        <v>0.9772502472799208</v>
       </c>
     </row>
     <row r="6">
@@ -641,13 +641,13 @@
         <v>0.7537810042347247</v>
       </c>
       <c r="H6" t="n">
-        <v>982</v>
+        <v>961</v>
       </c>
       <c r="I6" t="n">
-        <v>1.782214156079855</v>
+        <v>1.74410163339383</v>
       </c>
       <c r="J6" t="n">
-        <v>0.969147005444646</v>
+        <v>0.9685420447670902</v>
       </c>
     </row>
     <row r="7">
@@ -675,10 +675,10 @@
         <v>0.7433333333333333</v>
       </c>
       <c r="H7" t="n">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="I7" t="n">
-        <v>2.81</v>
+        <v>2.87</v>
       </c>
       <c r="J7" t="n">
         <v>1</v>
@@ -709,10 +709,10 @@
         <v>0.8699186991869918</v>
       </c>
       <c r="H8" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I8" t="n">
-        <v>2.51219512195122</v>
+        <v>2.536585365853659</v>
       </c>
       <c r="J8" t="n">
         <v>1</v>
@@ -743,10 +743,10 @@
         <v>0.8564476885644768</v>
       </c>
       <c r="H9" t="n">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="I9" t="n">
-        <v>1.948905109489051</v>
+        <v>1.91970802919708</v>
       </c>
       <c r="J9" t="n">
         <v>1</v>
@@ -777,13 +777,13 @@
         <v>0.7514450867052023</v>
       </c>
       <c r="H10" t="n">
-        <v>1338</v>
+        <v>1346</v>
       </c>
       <c r="I10" t="n">
-        <v>1.289017341040462</v>
+        <v>1.296724470134875</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9502247912652537</v>
+        <v>0.9473346178548491</v>
       </c>
     </row>
     <row r="11">
@@ -845,10 +845,10 @@
         <v>0.826530612244898</v>
       </c>
       <c r="H12" t="n">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I12" t="n">
-        <v>2.081632653061225</v>
+        <v>2.102040816326531</v>
       </c>
       <c r="J12" t="n">
         <v>1</v>
@@ -879,13 +879,13 @@
         <v>0.7219343696027634</v>
       </c>
       <c r="H13" t="n">
-        <v>1414</v>
+        <v>1409</v>
       </c>
       <c r="I13" t="n">
-        <v>1.221070811744387</v>
+        <v>1.216753022452504</v>
       </c>
       <c r="J13" t="n">
-        <v>0.927461139896373</v>
+        <v>0.9242947610823259</v>
       </c>
     </row>
     <row r="14">
@@ -904,22 +904,22 @@
         <v>811</v>
       </c>
       <c r="E14" t="n">
-        <v>1320</v>
+        <v>1027</v>
       </c>
       <c r="F14" t="n">
-        <v>1.627620221948212</v>
+        <v>1.266337854500617</v>
       </c>
       <c r="G14" t="n">
-        <v>0.8388820386354295</v>
+        <v>0.8947801068639539</v>
       </c>
       <c r="H14" t="n">
-        <v>1400</v>
+        <v>1114</v>
       </c>
       <c r="I14" t="n">
-        <v>1.726263871763255</v>
+        <v>1.373612823674476</v>
       </c>
       <c r="J14" t="n">
-        <v>0.9819153308672421</v>
+        <v>0.9905466502260584</v>
       </c>
     </row>
     <row r="15">
@@ -938,19 +938,19 @@
         <v>71</v>
       </c>
       <c r="E15" t="n">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="F15" t="n">
-        <v>2.394366197183099</v>
+        <v>2.126760563380282</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7605633802816901</v>
+        <v>0.7746478873239436</v>
       </c>
       <c r="H15" t="n">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="I15" t="n">
-        <v>2.436619718309859</v>
+        <v>2.056338028169014</v>
       </c>
       <c r="J15" t="n">
         <v>1</v>
@@ -981,13 +981,13 @@
         <v>0.8176100628930818</v>
       </c>
       <c r="H16" t="n">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="I16" t="n">
-        <v>2.113207547169811</v>
+        <v>2.128301886792453</v>
       </c>
       <c r="J16" t="n">
-        <v>0.9949685534591195</v>
+        <v>0.9974842767295597</v>
       </c>
     </row>
     <row r="17">
@@ -1015,13 +1015,13 @@
         <v>0.827485380116959</v>
       </c>
       <c r="H17" t="n">
-        <v>3767</v>
+        <v>3758</v>
       </c>
       <c r="I17" t="n">
-        <v>1.376827485380117</v>
+        <v>1.373538011695906</v>
       </c>
       <c r="J17" t="n">
-        <v>0.9512670565302144</v>
+        <v>0.9522417153996101</v>
       </c>
     </row>
     <row r="18">
@@ -1040,22 +1040,22 @@
         <v>3234</v>
       </c>
       <c r="E18" t="n">
-        <v>4819</v>
+        <v>4698</v>
       </c>
       <c r="F18" t="n">
-        <v>1.490105132962276</v>
+        <v>1.452690166975881</v>
       </c>
       <c r="G18" t="n">
-        <v>0.8531230674087817</v>
+        <v>0.8593073593073594</v>
       </c>
       <c r="H18" t="n">
-        <v>5278</v>
+        <v>4497</v>
       </c>
       <c r="I18" t="n">
-        <v>1.632034632034632</v>
+        <v>1.390538033395176</v>
       </c>
       <c r="J18" t="n">
-        <v>0.9466089466089466</v>
+        <v>0.9706246134817563</v>
       </c>
     </row>
     <row r="19">
@@ -1074,22 +1074,22 @@
         <v>423</v>
       </c>
       <c r="E19" t="n">
-        <v>543</v>
+        <v>507</v>
       </c>
       <c r="F19" t="n">
-        <v>1.283687943262411</v>
+        <v>1.198581560283688</v>
       </c>
       <c r="G19" t="n">
-        <v>0.8841607565011821</v>
+        <v>0.8912529550827423</v>
       </c>
       <c r="H19" t="n">
-        <v>583</v>
+        <v>541</v>
       </c>
       <c r="I19" t="n">
-        <v>1.378250591016549</v>
+        <v>1.278959810874704</v>
       </c>
       <c r="J19" t="n">
-        <v>0.9929078014184397</v>
+        <v>0.9976359338061466</v>
       </c>
     </row>
     <row r="20">
@@ -1108,19 +1108,19 @@
         <v>273</v>
       </c>
       <c r="E20" t="n">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="F20" t="n">
-        <v>1.981684981684982</v>
+        <v>1.93040293040293</v>
       </c>
       <c r="G20" t="n">
-        <v>0.9133089133089133</v>
+        <v>0.9157509157509157</v>
       </c>
       <c r="H20" t="n">
-        <v>460</v>
+        <v>435</v>
       </c>
       <c r="I20" t="n">
-        <v>1.684981684981685</v>
+        <v>1.593406593406593</v>
       </c>
       <c r="J20" t="n">
         <v>0.9987789987789988</v>
@@ -1151,13 +1151,13 @@
         <v>0.8326745718050066</v>
       </c>
       <c r="H21" t="n">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="I21" t="n">
-        <v>2.766798418972332</v>
+        <v>2.758893280632411</v>
       </c>
       <c r="J21" t="n">
-        <v>0.997364953886693</v>
+        <v>0.9960474308300395</v>
       </c>
     </row>
     <row r="22">
@@ -1219,10 +1219,10 @@
         <v>0.811965811965812</v>
       </c>
       <c r="H23" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I23" t="n">
-        <v>3.179487179487179</v>
+        <v>3.230769230769231</v>
       </c>
       <c r="J23" t="n">
         <v>1</v>
@@ -1253,10 +1253,10 @@
         <v>0.92</v>
       </c>
       <c r="H24" t="n">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I24" t="n">
-        <v>5.44</v>
+        <v>5.36</v>
       </c>
       <c r="J24" t="n">
         <v>1</v>
@@ -1287,13 +1287,13 @@
         <v>0.8538681948424068</v>
       </c>
       <c r="H25" t="n">
-        <v>1074</v>
+        <v>1063</v>
       </c>
       <c r="I25" t="n">
-        <v>3.077363896848138</v>
+        <v>3.045845272206304</v>
       </c>
       <c r="J25" t="n">
-        <v>0.9980897803247374</v>
+        <v>0.9923591212989494</v>
       </c>
     </row>
     <row r="26">
@@ -1321,13 +1321,13 @@
         <v>0.7945205479452054</v>
       </c>
       <c r="H26" t="n">
-        <v>277</v>
+        <v>298</v>
       </c>
       <c r="I26" t="n">
-        <v>3.794520547945206</v>
+        <v>4.082191780821918</v>
       </c>
       <c r="J26" t="n">
-        <v>1</v>
+        <v>0.9954337899543378</v>
       </c>
     </row>
     <row r="27">
@@ -1346,19 +1346,19 @@
         <v>181</v>
       </c>
       <c r="E27" t="n">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="F27" t="n">
-        <v>4.94475138121547</v>
+        <v>4.950276243093922</v>
       </c>
       <c r="G27" t="n">
-        <v>0.8121546961325967</v>
+        <v>0.8066298342541437</v>
       </c>
       <c r="H27" t="n">
-        <v>863</v>
+        <v>831</v>
       </c>
       <c r="I27" t="n">
-        <v>4.767955801104972</v>
+        <v>4.591160220994476</v>
       </c>
       <c r="J27" t="n">
         <v>1</v>
@@ -1389,13 +1389,13 @@
         <v>0.8026905829596412</v>
       </c>
       <c r="H28" t="n">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I28" t="n">
-        <v>1.426008968609865</v>
+        <v>1.42152466367713</v>
       </c>
       <c r="J28" t="n">
-        <v>0.9985052316890882</v>
+        <v>0.9955156950672646</v>
       </c>
     </row>
     <row r="29">
@@ -1423,10 +1423,10 @@
         <v>0.8282828282828283</v>
       </c>
       <c r="H29" t="n">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="I29" t="n">
-        <v>4.151515151515151</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="J29" t="n">
         <v>1</v>
@@ -1457,13 +1457,13 @@
         <v>0.8865248226950354</v>
       </c>
       <c r="H30" t="n">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="I30" t="n">
-        <v>3.627659574468085</v>
+        <v>3.542553191489362</v>
       </c>
       <c r="J30" t="n">
-        <v>1</v>
+        <v>0.9964539007092199</v>
       </c>
     </row>
     <row r="31">
@@ -1491,10 +1491,10 @@
         <v>0.9333333333333333</v>
       </c>
       <c r="H31" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I31" t="n">
-        <v>1.333333333333333</v>
+        <v>1.466666666666667</v>
       </c>
       <c r="J31" t="n">
         <v>1</v>
@@ -1525,10 +1525,10 @@
         <v>0.8888888888888888</v>
       </c>
       <c r="H32" t="n">
-        <v>1406</v>
+        <v>1327</v>
       </c>
       <c r="I32" t="n">
-        <v>36.05128205128205</v>
+        <v>34.02564102564103</v>
       </c>
       <c r="J32" t="n">
         <v>1</v>
@@ -1559,10 +1559,10 @@
         <v>0.8601190476190477</v>
       </c>
       <c r="H33" t="n">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="I33" t="n">
-        <v>4.098214285714286</v>
+        <v>4.017857142857143</v>
       </c>
       <c r="J33" t="n">
         <v>1</v>
@@ -1584,19 +1584,19 @@
         <v>94</v>
       </c>
       <c r="E34" t="n">
-        <v>2852</v>
+        <v>1559</v>
       </c>
       <c r="F34" t="n">
-        <v>30.34042553191489</v>
+        <v>16.58510638297872</v>
       </c>
       <c r="G34" t="n">
-        <v>0.8829787234042553</v>
+        <v>0.8723404255319149</v>
       </c>
       <c r="H34" t="n">
-        <v>2333</v>
+        <v>1538</v>
       </c>
       <c r="I34" t="n">
-        <v>24.81914893617021</v>
+        <v>16.36170212765957</v>
       </c>
       <c r="J34" t="n">
         <v>1</v>
@@ -1627,10 +1627,10 @@
         <v>0.7716535433070866</v>
       </c>
       <c r="H35" t="n">
-        <v>982</v>
+        <v>954</v>
       </c>
       <c r="I35" t="n">
-        <v>7.732283464566929</v>
+        <v>7.511811023622047</v>
       </c>
       <c r="J35" t="n">
         <v>1</v>
@@ -1661,10 +1661,10 @@
         <v>0.8045977011494253</v>
       </c>
       <c r="H36" t="n">
-        <v>854</v>
+        <v>893</v>
       </c>
       <c r="I36" t="n">
-        <v>29.44827586206896</v>
+        <v>30.79310344827586</v>
       </c>
       <c r="J36" t="n">
         <v>1</v>
@@ -1695,10 +1695,10 @@
         <v>0.9308176100628931</v>
       </c>
       <c r="H37" t="n">
-        <v>808</v>
+        <v>819</v>
       </c>
       <c r="I37" t="n">
-        <v>15.24528301886792</v>
+        <v>15.45283018867925</v>
       </c>
       <c r="J37" t="n">
         <v>1</v>
@@ -1729,13 +1729,13 @@
         <v>0.8096906012842966</v>
       </c>
       <c r="H38" t="n">
-        <v>1405</v>
+        <v>1384</v>
       </c>
       <c r="I38" t="n">
-        <v>2.460595446584939</v>
+        <v>2.423817863397548</v>
       </c>
       <c r="J38" t="n">
-        <v>0.9772329246935202</v>
+        <v>0.978984238178634</v>
       </c>
     </row>
     <row r="39">
@@ -1763,10 +1763,10 @@
         <v>0.8707482993197279</v>
       </c>
       <c r="H39" t="n">
-        <v>256</v>
+        <v>217</v>
       </c>
       <c r="I39" t="n">
-        <v>5.224489795918367</v>
+        <v>4.428571428571429</v>
       </c>
       <c r="J39" t="n">
         <v>1</v>
@@ -1797,10 +1797,10 @@
         <v>0.9057239057239057</v>
       </c>
       <c r="H40" t="n">
-        <v>1343</v>
+        <v>1330</v>
       </c>
       <c r="I40" t="n">
-        <v>13.56565656565657</v>
+        <v>13.43434343434343</v>
       </c>
       <c r="J40" t="n">
         <v>1</v>
@@ -1831,10 +1831,10 @@
         <v>0.9583333333333334</v>
       </c>
       <c r="H41" t="n">
-        <v>350</v>
+        <v>307</v>
       </c>
       <c r="I41" t="n">
-        <v>14.58333333333333</v>
+        <v>12.79166666666667</v>
       </c>
       <c r="J41" t="n">
         <v>1</v>
@@ -1856,19 +1856,19 @@
         <v>189</v>
       </c>
       <c r="E42" t="n">
-        <v>2104</v>
+        <v>1810</v>
       </c>
       <c r="F42" t="n">
-        <v>11.13227513227513</v>
+        <v>9.576719576719576</v>
       </c>
       <c r="G42" t="n">
-        <v>0.9259259259259259</v>
+        <v>0.9435626102292769</v>
       </c>
       <c r="H42" t="n">
-        <v>1701</v>
+        <v>1355</v>
       </c>
       <c r="I42" t="n">
-        <v>9</v>
+        <v>7.169312169312169</v>
       </c>
       <c r="J42" t="n">
         <v>1</v>
@@ -1899,10 +1899,10 @@
         <v>1</v>
       </c>
       <c r="H43" t="n">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="I43" t="n">
-        <v>29.125</v>
+        <v>25.625</v>
       </c>
       <c r="J43" t="n">
         <v>1</v>
@@ -1933,10 +1933,10 @@
         <v>0.9354838709677419</v>
       </c>
       <c r="H44" t="n">
-        <v>2284</v>
+        <v>2456</v>
       </c>
       <c r="I44" t="n">
-        <v>73.6774193548387</v>
+        <v>79.2258064516129</v>
       </c>
       <c r="J44" t="n">
         <v>1</v>
@@ -1967,10 +1967,10 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="H45" t="n">
-        <v>1107</v>
+        <v>1121</v>
       </c>
       <c r="I45" t="n">
-        <v>61.5</v>
+        <v>62.27777777777778</v>
       </c>
       <c r="J45" t="n">
         <v>1</v>

</xml_diff>